<commit_message>
major: first rendering of dashboard
</commit_message>
<xml_diff>
--- a/data/4-11-2021_Game_1.xlsx
+++ b/data/4-11-2021_Game_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanuel.woldekidan/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanuel.woldekidan/gitrepos/flamingo_stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5EF93E-536C-C84E-BB31-051339B395F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A02DD14-9B6C-424D-B484-91714BE34297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="3" xr2:uid="{09AF5A8C-78D4-2142-A69D-63FA30327E3F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{09AF5A8C-78D4-2142-A69D-63FA30327E3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="1" r:id="rId1"/>
@@ -38,13 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="38">
-  <si>
-    <t>Team A</t>
-  </si>
-  <si>
-    <t>Team B</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>Flamingo Fadaways</t>
   </si>
@@ -152,6 +146,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -226,6 +229,7 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,7 +547,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -555,31 +559,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
       <c r="B1" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="C2" s="2">
         <v>15</v>
@@ -598,11 +605,11 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="C3" s="2">
         <v>33</v>
@@ -642,28 +649,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -671,10 +678,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2">
         <v>7</v>
@@ -691,10 +698,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -707,10 +714,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2">
         <v>30</v>
@@ -725,10 +732,10 @@
         <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2">
         <v>6</v>
@@ -747,10 +754,10 @@
         <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2">
         <v>12</v>
@@ -771,10 +778,10 @@
         <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -813,28 +820,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -842,7 +849,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -856,10 +863,10 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2">
         <v>28</v>
@@ -874,10 +881,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2">
         <v>18</v>
@@ -892,10 +899,10 @@
         <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="2">
         <v>18</v>
@@ -912,10 +919,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -928,10 +935,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2">
         <v>26</v>
@@ -948,10 +955,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -968,10 +975,10 @@
         <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2">
         <v>9</v>
@@ -995,7 +1002,7 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1009,19 +1016,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1104,7 +1111,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1205,7 +1212,7 @@
         <v>34</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1387,7 +1394,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1407,7 +1414,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1577,7 +1584,7 @@
         <v>22</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="2"/>
@@ -1621,7 +1628,7 @@
         <v>9</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="2"/>
@@ -1711,7 +1718,7 @@
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="2"/>
@@ -1838,7 +1845,7 @@
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="2"/>
@@ -1849,7 +1856,7 @@
         <v>41</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="2"/>
@@ -1893,7 +1900,7 @@
         <v>22</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C78" s="3">
         <v>28</v>
@@ -1904,7 +1911,7 @@
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="2"/>
@@ -1927,7 +1934,7 @@
       <c r="C81" s="3"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
WIP: building nicer rundown
</commit_message>
<xml_diff>
--- a/data/4-11-2021_Game_1.xlsx
+++ b/data/4-11-2021_Game_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanuel.woldekidan/gitrepos/flamingo_stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A02DD14-9B6C-424D-B484-91714BE34297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC057FB-6C9B-B54F-BB2D-FE28EE9365AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{09AF5A8C-78D4-2142-A69D-63FA30327E3F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="3" xr2:uid="{09AF5A8C-78D4-2142-A69D-63FA30327E3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="1" r:id="rId1"/>
@@ -61,15 +61,9 @@
     <t>Final</t>
   </si>
   <si>
-    <t>Nummer</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Gespielt</t>
-  </si>
-  <si>
     <t>1. Foul</t>
   </si>
   <si>
@@ -133,18 +127,6 @@
     <t>Minute</t>
   </si>
   <si>
-    <t>A Nummer</t>
-  </si>
-  <si>
-    <t>A Score</t>
-  </si>
-  <si>
-    <t>B Nummer</t>
-  </si>
-  <si>
-    <t>B Score</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -155,6 +137,24 @@
   </si>
   <si>
     <t>B</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Played</t>
+  </si>
+  <si>
+    <t># A</t>
+  </si>
+  <si>
+    <t>Score A</t>
+  </si>
+  <si>
+    <t># B</t>
+  </si>
+  <si>
+    <t>Score B</t>
   </si>
 </sst>
 </file>
@@ -560,10 +560,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>2</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -606,7 +606,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -637,7 +637,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -649,28 +649,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -678,10 +678,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2">
         <v>7</v>
@@ -698,10 +698,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -714,10 +714,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2">
         <v>30</v>
@@ -732,10 +732,10 @@
         <v>22</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2">
         <v>6</v>
@@ -754,10 +754,10 @@
         <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2">
         <v>12</v>
@@ -778,10 +778,10 @@
         <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2">
         <v>1</v>
@@ -807,7 +807,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -820,28 +820,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -849,7 +849,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -863,10 +863,10 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2">
         <v>28</v>
@@ -881,10 +881,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2">
         <v>18</v>
@@ -899,10 +899,10 @@
         <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2">
         <v>18</v>
@@ -919,10 +919,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -935,10 +935,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2">
         <v>26</v>
@@ -955,10 +955,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2">
         <v>1</v>
@@ -975,10 +975,10 @@
         <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2">
         <v>9</v>
@@ -1002,33 +1002,33 @@
   <dimension ref="A1:E97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1111,7 +1111,7 @@
       <c r="C8" s="3"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1212,7 +1212,7 @@
         <v>34</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1394,7 +1394,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1414,7 +1414,7 @@
       <c r="C35" s="3"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1584,7 +1584,7 @@
         <v>22</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="2"/>
@@ -1628,7 +1628,7 @@
         <v>9</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="2"/>
@@ -1718,7 +1718,7 @@
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="2"/>
@@ -1845,7 +1845,7 @@
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="2"/>
@@ -1856,7 +1856,7 @@
         <v>41</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="2"/>
@@ -1900,7 +1900,7 @@
         <v>22</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C78" s="3">
         <v>28</v>
@@ -1911,7 +1911,7 @@
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="2"/>
       <c r="B79" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="2"/>
@@ -1934,7 +1934,7 @@
       <c r="C81" s="3"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
BUG: fix errors in data
</commit_message>
<xml_diff>
--- a/data/4-11-2021_Game_1.xlsx
+++ b/data/4-11-2021_Game_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amanuel.woldekidan/gitrepos/flamingo_stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC057FB-6C9B-B54F-BB2D-FE28EE9365AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F16C07C-B032-254C-8C90-FEFFD801EEF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" activeTab="3" xr2:uid="{09AF5A8C-78D4-2142-A69D-63FA30327E3F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="28300" activeTab="3" xr2:uid="{09AF5A8C-78D4-2142-A69D-63FA30327E3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="1" r:id="rId1"/>
@@ -1001,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0A9B0DD-A295-D744-9B94-C8207D40001D}">
   <dimension ref="A1:E97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1467,7 +1467,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B40" s="2">
         <v>21</v>
@@ -1562,7 +1562,7 @@
         <v>17</v>
       </c>
       <c r="D48" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E48" s="2">
         <v>57</v>

</xml_diff>